<commit_message>
Added link (SP) and status
</commit_message>
<xml_diff>
--- a/Potential Companies.xlsx
+++ b/Potential Companies.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8025"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
   <si>
     <t>Company</t>
   </si>
@@ -150,12 +150,21 @@
   </si>
   <si>
     <t>24.11.2015</t>
+  </si>
+  <si>
+    <t>http://www.sp.se/en/workatsp/students/masterthesis/Sidor/STRATEGIESANDMETHODSFORSUSTAINABLEINNOVATIONANDTRANSFORMATION.aspx</t>
+  </si>
+  <si>
+    <t>What have we done?</t>
+  </si>
+  <si>
+    <t>Sent mail, waiting for answer.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -217,6 +226,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -264,7 +276,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -299,7 +311,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -508,18 +520,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F9:F10"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -550,8 +563,11 @@
       <c r="K1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -580,7 +596,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -609,7 +625,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -629,7 +645,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -649,13 +665,16 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
       <c r="I6" t="s">
         <v>34</v>
       </c>
@@ -665,8 +684,11 @@
       <c r="K6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -686,7 +708,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -703,7 +725,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -717,7 +739,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -725,7 +747,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -738,8 +760,11 @@
       <c r="J11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>

</xml_diff>